<commit_message>
Finalizes creation of json files as a step in submission packages procedure
</commit_message>
<xml_diff>
--- a/requests/ECHO_HIV_HI_PBMC_csrna-seq_withoutProjectName.xlsx
+++ b/requests/ECHO_HIV_HI_PBMC_csrna-seq_withoutProjectName.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MounSinai\Darpa\Programming\submission\requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FA63D4-7D57-42B6-97E5-634E45C191AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0334B4CB-55E3-42BC-985D-E4C24D47AC48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1022EA94-C927-47D4-994A-3445E7764CD5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
   <si>
     <t>Project</t>
   </si>
@@ -223,12 +223,6 @@
   </si>
   <si>
     <t>Sample_id</t>
-  </si>
-  <si>
-    <t>Experiment_id</t>
-  </si>
-  <si>
-    <t>Exp_123</t>
   </si>
   <si>
     <t>AS17-00144</t>
@@ -601,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{648F6FB2-DCD5-4DC2-9468-8A496EE9201E}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,10 +607,9 @@
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -635,11 +628,8 @@
       <c r="F1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -656,13 +646,10 @@
         <v>58</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
         <v>59</v>
       </c>
@@ -670,7 +657,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
         <v>60</v>
       </c>
@@ -678,7 +665,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F5" s="1"/>
     </row>
   </sheetData>

</xml_diff>